<commit_message>
update calc method of baudrate I2C
</commit_message>
<xml_diff>
--- a/Other/Calc BaudrateConfig.xlsx
+++ b/Other/Calc BaudrateConfig.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Fosc</t>
   </si>
@@ -38,6 +38,12 @@
   <si>
     <t>I2C</t>
   </si>
+  <si>
+    <t>Baudrate = 9600 bd/s</t>
+  </si>
+  <si>
+    <t>38400 bd/s</t>
+  </si>
 </sst>
 </file>
 
@@ -56,7 +62,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +93,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -100,16 +112,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,420 +436,723 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3">
-        <f>A3*10^6/(9600*16*4)-1</f>
-        <v>12.020833333333334</v>
-      </c>
-      <c r="D3" s="4">
-        <f>A3*10^6*4/(9600*16*4)-1</f>
-        <v>51.083333333333336</v>
-      </c>
-      <c r="E3" s="5">
-        <f>A3*10^6*8/(9600*16*4)-1</f>
-        <v>103.16666666666667</v>
-      </c>
-      <c r="F3" s="6">
-        <f>A3*10^6*16/(9600*16*4)-1</f>
-        <v>207.33333333333334</v>
-      </c>
-      <c r="H3" s="3">
-        <f>A3*10^6*(1/9600 - 1/1111111)-1</f>
-        <v>825.13333261333332</v>
-      </c>
-      <c r="I3" s="4">
-        <f>A3*10^6*4*(1/9600 - 1/1111111)-1</f>
-        <v>3303.5333304533333</v>
-      </c>
-      <c r="J3" s="5">
-        <f>A3*10^6*8*(1/9600 - 1/1111111)-1</f>
-        <v>6608.0666609066666</v>
-      </c>
-      <c r="K3" s="6">
-        <f>A3*10^6*16*(1/9600 - 1/1111111)-1</f>
-        <v>13217.133321813333</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>7.3727999999999998</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3">
-        <f t="shared" ref="C4:C12" si="0">A4*10^6/(9600*16*4)-1</f>
-        <v>11</v>
-      </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D12" si="1">A4*10^6*4/(9600*16*4)-1</f>
-        <v>47</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" ref="E4:E12" si="2">A4*10^6*8/(9600*16*4)-1</f>
-        <v>95</v>
-      </c>
-      <c r="F4" s="6">
-        <f t="shared" ref="F4:F12" si="3">A4*10^6*16/(9600*16*4)-1</f>
-        <v>191</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" ref="H4:H12" si="4">A4*10^6*(1/9600 - 1/1111111)-1</f>
-        <v>760.36447933644797</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" ref="I4:I12" si="5">A4*10^6*4*(1/9600 - 1/1111111)-1</f>
-        <v>3044.4579173457919</v>
-      </c>
-      <c r="J4" s="5">
-        <f t="shared" ref="J4:J12" si="6">A4*10^6*8*(1/9600 - 1/1111111)-1</f>
-        <v>6089.9158346915838</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" ref="K4:K12" si="7">A4*10^6*16*(1/9600 - 1/1111111)-1</f>
-        <v>12180.831669383168</v>
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <f>A4*10^6/(9600*16*4)-1</f>
+        <v>5.510416666666667</v>
+      </c>
+      <c r="D4" s="3">
+        <f>A4*10^6*4/(9600*16*4)-1</f>
+        <v>25.041666666666668</v>
+      </c>
+      <c r="E4" s="4">
+        <f>A4*10^6*8/(9600*16*4)-1</f>
+        <v>51.083333333333336</v>
+      </c>
+      <c r="F4" s="5">
+        <f>A4*10^6*16/(9600*16*4)-1</f>
+        <v>103.16666666666667</v>
+      </c>
+      <c r="H4" s="2">
+        <f>A4*10^6*(1/100000 - 1/1111111)/4-1</f>
+        <v>8.0999999099999922</v>
+      </c>
+      <c r="I4" s="3">
+        <f>A4*10^6*4*(1/100000 - 1/1111111)/4-1</f>
+        <v>35.399999639999969</v>
+      </c>
+      <c r="J4" s="4">
+        <f>A4*10^6*8*(1/100000 - 1/1111111)/4-1</f>
+        <v>71.799999279999938</v>
+      </c>
+      <c r="K4" s="5">
+        <f>A4*10^6*16*(1/100000 - 1/1111111)/4-1</f>
+        <v>144.59999855999988</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
-        <f t="shared" si="0"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2">
+        <f t="shared" ref="C5:C23" si="0">A5*10^6/(9600*16*4)-1</f>
         <v>8.765625</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" si="1"/>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D23" si="1">A5*10^6*4/(9600*16*4)-1</f>
         <v>38.0625</v>
       </c>
-      <c r="E5" s="5">
-        <f t="shared" si="2"/>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E23" si="2">A5*10^6*8/(9600*16*4)-1</f>
         <v>77.125</v>
       </c>
-      <c r="F5" s="6">
-        <f t="shared" si="3"/>
+      <c r="F5" s="5">
+        <f t="shared" ref="F5:F23" si="3">A5*10^6*16/(9600*16*4)-1</f>
         <v>155.25</v>
       </c>
-      <c r="H5" s="3">
-        <f t="shared" si="4"/>
-        <v>618.59999945999994</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="5"/>
-        <v>2477.3999978399997</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" si="6"/>
-        <v>4955.7999956799995</v>
-      </c>
-      <c r="K5" s="6">
-        <f t="shared" si="7"/>
-        <v>9912.599991359999</v>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H23" si="4">A5*10^6*(1/100000 - 1/1111111)/4-1</f>
+        <v>12.649999864999989</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" ref="I5:I23" si="5">A5*10^6*4*(1/100000 - 1/1111111)/4-1</f>
+        <v>53.599999459999957</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J23" si="6">A5*10^6*8*(1/100000 - 1/1111111)/4-1</f>
+        <v>108.19999891999991</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ref="K5:K23" si="7">A5*10^6*16*(1/100000 - 1/1111111)/4-1</f>
+        <v>217.39999783999983</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3">
+        <v>7.3727999999999998</v>
+      </c>
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>5.510416666666667</v>
-      </c>
-      <c r="D6" s="4">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>25.041666666666668</v>
-      </c>
-      <c r="E6" s="5">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4">
         <f t="shared" si="2"/>
-        <v>51.083333333333336</v>
-      </c>
-      <c r="F6" s="6">
+        <v>95</v>
+      </c>
+      <c r="F6" s="5">
         <f t="shared" si="3"/>
-        <v>103.16666666666667</v>
-      </c>
-      <c r="H6" s="3">
+        <v>191</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="4"/>
-        <v>412.06666630666666</v>
-      </c>
-      <c r="I6" s="4">
+        <v>15.773119834111984</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="5"/>
-        <v>1651.2666652266666</v>
-      </c>
-      <c r="J6" s="5">
+        <v>66.092479336447937</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="6"/>
-        <v>3303.5333304533333</v>
-      </c>
-      <c r="K6" s="6">
+        <v>133.18495867289587</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>6608.0666609066666</v>
+        <v>267.36991734579175</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>32.768000000000001</v>
-      </c>
-      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>52.333333333333336</v>
-      </c>
-      <c r="D7" s="4">
+        <v>12.020833333333334</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>212.33333333333334</v>
-      </c>
-      <c r="E7" s="5">
+        <v>51.083333333333336</v>
+      </c>
+      <c r="E7" s="4">
         <f t="shared" si="2"/>
-        <v>425.66666666666669</v>
-      </c>
-      <c r="F7" s="6">
+        <v>103.16666666666667</v>
+      </c>
+      <c r="F7" s="5">
         <f t="shared" si="3"/>
-        <v>852.33333333333337</v>
-      </c>
-      <c r="H7" s="3">
+        <v>207.33333333333334</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="4"/>
-        <v>3382.8421303842133</v>
-      </c>
-      <c r="I7" s="4">
+        <v>17.199999819999984</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="5"/>
-        <v>13534.368521536853</v>
-      </c>
-      <c r="J7" s="5">
+        <v>71.799999279999938</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="6"/>
-        <v>27069.737043073706</v>
-      </c>
-      <c r="K7" s="6">
+        <v>144.59999855999988</v>
+      </c>
+      <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>54140.474086147413</v>
+        <v>290.19999711999975</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3">
+        <v>11.059200000000001</v>
+      </c>
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>39.690104166666664</v>
-      </c>
-      <c r="D8" s="4">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>161.76041666666666</v>
-      </c>
-      <c r="E8" s="5">
+        <v>71</v>
+      </c>
+      <c r="E8" s="4">
         <f t="shared" si="2"/>
-        <v>324.52083333333331</v>
-      </c>
-      <c r="F8" s="6">
+        <v>143</v>
+      </c>
+      <c r="F8" s="5">
         <f t="shared" si="3"/>
-        <v>650.04166666666663</v>
-      </c>
-      <c r="H8" s="3">
+        <v>287</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="4"/>
-        <v>2580.6666644166667</v>
-      </c>
-      <c r="I8" s="4">
+        <v>24.159679751167978</v>
+      </c>
+      <c r="I8" s="3">
         <f t="shared" si="5"/>
-        <v>10325.666657666667</v>
-      </c>
-      <c r="J8" s="5">
+        <v>99.638719004671913</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" si="6"/>
-        <v>20652.333315333333</v>
-      </c>
-      <c r="K8" s="6">
+        <v>200.27743800934383</v>
+      </c>
+      <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>41305.666630666667</v>
+        <v>401.55487601868765</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>38.0625</v>
-      </c>
-      <c r="D9" s="4">
+        <v>18.53125</v>
+      </c>
+      <c r="D9" s="3">
         <f t="shared" si="1"/>
+        <v>77.125</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="2"/>
         <v>155.25</v>
       </c>
-      <c r="E9" s="5">
-        <f t="shared" si="2"/>
+      <c r="F9" s="5">
+        <f t="shared" si="3"/>
         <v>311.5</v>
       </c>
-      <c r="F9" s="6">
-        <f t="shared" si="3"/>
-        <v>624</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <f t="shared" si="4"/>
-        <v>2477.3999978399997</v>
-      </c>
-      <c r="I9" s="4">
+        <v>26.299999729999978</v>
+      </c>
+      <c r="I9" s="3">
         <f t="shared" si="5"/>
-        <v>9912.599991359999</v>
-      </c>
-      <c r="J9" s="5">
+        <v>108.19999891999991</v>
+      </c>
+      <c r="J9" s="4">
         <f t="shared" si="6"/>
-        <v>19826.199982719998</v>
-      </c>
-      <c r="K9" s="6">
+        <v>217.39999783999983</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>39653.399965439996</v>
+        <v>435.79999567999965</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>20</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>31.552083333333336</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" si="1"/>
         <v>129.20833333333334</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="2"/>
         <v>259.41666666666669</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="3"/>
         <v>519.83333333333337</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <f t="shared" si="4"/>
-        <v>2064.3333315333334</v>
-      </c>
-      <c r="I10" s="4">
+        <v>44.499999549999963</v>
+      </c>
+      <c r="I10" s="3">
         <f t="shared" si="5"/>
-        <v>8260.3333261333337</v>
-      </c>
-      <c r="J10" s="5">
+        <v>180.99999819999985</v>
+      </c>
+      <c r="J10" s="4">
         <f t="shared" si="6"/>
-        <v>16521.666652266667</v>
-      </c>
-      <c r="K10" s="6">
+        <v>362.9999963999997</v>
+      </c>
+      <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>33044.333304533335</v>
+        <v>726.9999927999994</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>18.53125</v>
-      </c>
-      <c r="D11" s="4">
+        <v>38.0625</v>
+      </c>
+      <c r="D11" s="3">
         <f t="shared" si="1"/>
-        <v>77.125</v>
-      </c>
-      <c r="E11" s="5">
+        <v>155.25</v>
+      </c>
+      <c r="E11" s="4">
         <f t="shared" si="2"/>
-        <v>155.25</v>
-      </c>
-      <c r="F11" s="6">
+        <v>311.5</v>
+      </c>
+      <c r="F11" s="5">
         <f t="shared" si="3"/>
-        <v>311.5</v>
-      </c>
-      <c r="H11" s="3">
+        <v>624</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="4"/>
-        <v>1238.1999989199999</v>
-      </c>
-      <c r="I11" s="4">
+        <v>53.599999459999957</v>
+      </c>
+      <c r="I11" s="3">
         <f t="shared" si="5"/>
-        <v>4955.7999956799995</v>
-      </c>
-      <c r="J11" s="5">
+        <v>217.39999783999983</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="6"/>
-        <v>9912.599991359999</v>
-      </c>
-      <c r="K11" s="6">
+        <v>435.79999567999965</v>
+      </c>
+      <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>19826.199982719998</v>
+        <v>872.59999135999931</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>39.690104166666664</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>161.76041666666666</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="2"/>
+        <v>324.52083333333331</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="3"/>
+        <v>650.04166666666663</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="4"/>
+        <v>55.874999437499952</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="5"/>
+        <v>226.49999774999981</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="6"/>
+        <v>453.99999549999961</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="7"/>
+        <v>908.99999099999923</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>52.333333333333336</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>212.33333333333334</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>425.66666666666669</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="3"/>
+        <v>852.33333333333337</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="4"/>
+        <v>73.547199262719943</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="5"/>
+        <v>297.18879705087977</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="6"/>
+        <v>595.37759410175954</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="7"/>
+        <v>1191.7551882035191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>51.083333333333336</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>207.33333333333334</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="2"/>
+        <v>415.66666666666669</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="3"/>
+        <v>832.33333333333337</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="4"/>
+        <v>71.799999279999938</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="5"/>
+        <v>290.19999711999975</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="6"/>
+        <v>581.3999942399995</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="7"/>
+        <v>1163.799988479999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <f>A17*10^6/(38400*16*4)-1</f>
+        <v>0.62760416666666674</v>
+      </c>
+      <c r="D17" s="3">
+        <f>A17*10^6*4/(38400*16*4)-1</f>
+        <v>5.510416666666667</v>
+      </c>
+      <c r="E17" s="4">
+        <f>A17*10^6*8/(38400*16*4)-1</f>
+        <v>12.020833333333334</v>
+      </c>
+      <c r="F17" s="5">
+        <f>A17*10^6*16/(38400*16*4)-1</f>
+        <v>25.041666666666668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:C27" si="8">A18*10^6/(38400*16*4)-1</f>
+        <v>1.44140625</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" ref="D18:D27" si="9">A18*10^6*4/(38400*16*4)-1</f>
+        <v>8.765625</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" ref="E18:E27" si="10">A18*10^6*8/(38400*16*4)-1</f>
+        <v>18.53125</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" ref="F18:F27" si="11">A18*10^6*16/(38400*16*4)-1</f>
+        <v>38.0625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>7.3727999999999998</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="10"/>
+        <v>23</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="11"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="8"/>
+        <v>2.2552083333333335</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="9"/>
+        <v>12.020833333333334</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="10"/>
+        <v>25.041666666666668</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="11"/>
+        <v>51.083333333333336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>11.059200000000001</v>
       </c>
-      <c r="C12" s="3">
-        <f t="shared" si="0"/>
+      <c r="C21" s="2">
+        <f t="shared" si="8"/>
+        <v>3.5</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="D12" s="4">
-        <f t="shared" si="1"/>
+      <c r="E21" s="4">
+        <f t="shared" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="11"/>
         <v>71</v>
       </c>
-      <c r="E12" s="5">
-        <f t="shared" si="2"/>
-        <v>143</v>
-      </c>
-      <c r="F12" s="6">
-        <f t="shared" si="3"/>
-        <v>287</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="4"/>
-        <v>1141.046719004672</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="5"/>
-        <v>4567.1868760186881</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="6"/>
-        <v>9135.3737520373761</v>
-      </c>
-      <c r="K12" s="6">
-        <f t="shared" si="7"/>
-        <v>18271.747504074752</v>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="8"/>
+        <v>3.8828125</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="9"/>
+        <v>18.53125</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="10"/>
+        <v>38.0625</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="11"/>
+        <v>77.125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="8"/>
+        <v>7.1380208333333339</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="9"/>
+        <v>31.552083333333336</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="10"/>
+        <v>64.104166666666671</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="11"/>
+        <v>129.20833333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="8"/>
+        <v>8.765625</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="9"/>
+        <v>38.0625</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="10"/>
+        <v>77.125</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="11"/>
+        <v>155.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="8"/>
+        <v>9.1725260416666661</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="9"/>
+        <v>39.690104166666664</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="10"/>
+        <v>80.380208333333329</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="11"/>
+        <v>161.76041666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="8"/>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="9"/>
+        <v>52.333333333333336</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="10"/>
+        <v>105.66666666666667</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="11"/>
+        <v>212.33333333333334</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="8"/>
+        <v>12.020833333333334</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="9"/>
+        <v>51.083333333333336</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="10"/>
+        <v>103.16666666666667</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="11"/>
+        <v>207.33333333333334</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:A12">
+    <sortCondition ref="A3"/>
+  </sortState>
   <mergeCells count="2">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="H1:K1"/>

</xml_diff>

<commit_message>
update baudrate = 100000 bd/s of I2C
</commit_message>
<xml_diff>
--- a/Other/Calc BaudrateConfig.xlsx
+++ b/Other/Calc BaudrateConfig.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Fosc</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>38400 bd/s</t>
+  </si>
+  <si>
+    <t>Baudrate = 100000 bd/s</t>
   </si>
 </sst>
 </file>
@@ -119,11 +122,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,33 +439,35 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -536,35 +541,35 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C23" si="0">A5*10^6/(9600*16*4)-1</f>
+        <f t="shared" ref="C5:C14" si="0">A5*10^6/(9600*16*4)-1</f>
         <v>8.765625</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D23" si="1">A5*10^6*4/(9600*16*4)-1</f>
+        <f t="shared" ref="D5:D14" si="1">A5*10^6*4/(9600*16*4)-1</f>
         <v>38.0625</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E23" si="2">A5*10^6*8/(9600*16*4)-1</f>
+        <f t="shared" ref="E5:E14" si="2">A5*10^6*8/(9600*16*4)-1</f>
         <v>77.125</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F23" si="3">A5*10^6*16/(9600*16*4)-1</f>
+        <f t="shared" ref="F5:F14" si="3">A5*10^6*16/(9600*16*4)-1</f>
         <v>155.25</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ref="H5:H23" si="4">A5*10^6*(1/100000 - 1/1111111)/4-1</f>
+        <f t="shared" ref="H5:H14" si="4">A5*10^6*(1/100000 - 1/1111111)/4-1</f>
         <v>12.649999864999989</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" ref="I5:I23" si="5">A5*10^6*4*(1/100000 - 1/1111111)/4-1</f>
+        <f t="shared" ref="I5:I14" si="5">A5*10^6*4*(1/100000 - 1/1111111)/4-1</f>
         <v>53.599999459999957</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J23" si="6">A5*10^6*8*(1/100000 - 1/1111111)/4-1</f>
+        <f t="shared" ref="J5:J14" si="6">A5*10^6*8*(1/100000 - 1/1111111)/4-1</f>
         <v>108.19999891999991</v>
       </c>
       <c r="K5" s="5">
-        <f t="shared" ref="K5:K23" si="7">A5*10^6*16*(1/100000 - 1/1111111)/4-1</f>
+        <f t="shared" ref="K5:K14" si="7">A5*10^6*16*(1/100000 - 1/1111111)/4-1</f>
         <v>217.39999783999983</v>
       </c>
     </row>
@@ -902,21 +907,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">

</xml_diff>

<commit_message>
update baudrate error percent
</commit_message>
<xml_diff>
--- a/Other/Calc BaudrateConfig.xlsx
+++ b/Other/Calc BaudrateConfig.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Fosc</t>
   </si>
@@ -47,6 +47,9 @@
   <si>
     <t>Baudrate = 100000 bd/s</t>
   </si>
+  <si>
+    <t>% Error</t>
+  </si>
 </sst>
 </file>
 
@@ -55,10 +58,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -115,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -127,6 +138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,31 +443,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="14" max="14" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="8"/>
+      <c r="L1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="8"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
@@ -462,43 +488,75 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="M3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="O3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="Q3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S3" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -506,36 +564,68 @@
         <f>A4*10^6/(9600*16*4)-1</f>
         <v>5.510416666666667</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="10">
+        <f>ABS(A4*10^6/(16*4*(ROUND(C4,0)+1))-9600)*100/9600</f>
+        <v>6.9940476190476115</v>
+      </c>
+      <c r="E4" s="3">
         <f>A4*10^6*4/(9600*16*4)-1</f>
         <v>25.041666666666668</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="10">
+        <f>ABS(A4*10^6*4/(16*4*(ROUND(E4,0)+1))-9600)*100/9600</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G4" s="4">
         <f>A4*10^6*8/(9600*16*4)-1</f>
         <v>51.083333333333336</v>
       </c>
-      <c r="F4" s="5">
+      <c r="H4" s="10">
+        <f>ABS(A4*10^6*8/(16*4*(ROUND(G4,0)+1))-9600)*100/9600</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I4" s="5">
         <f>A4*10^6*16/(9600*16*4)-1</f>
         <v>103.16666666666667</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="10">
+        <f>ABS(A4*10^6*16/(16*4*(ROUND(I4,0)+1))-9600)*100/9600</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="L4" s="2">
         <f>A4*10^6*(1/100000 - 1/1111111)/4-1</f>
         <v>8.0999999099999922</v>
       </c>
-      <c r="I4" s="3">
+      <c r="M4" s="10">
+        <f>ABS(((4*(ROUND(L4,0)+1)/(A4*10^6)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.99999909999992154</v>
+      </c>
+      <c r="N4" s="3">
         <f>A4*10^6*4*(1/100000 - 1/1111111)/4-1</f>
         <v>35.399999639999969</v>
       </c>
-      <c r="J4" s="4">
+      <c r="O4" s="10">
+        <f>ABS(((4*(ROUND(N4,0)+1)/(A4*10^6*4)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.99999909999992154</v>
+      </c>
+      <c r="P4" s="4">
         <f>A4*10^6*8*(1/100000 - 1/1111111)/4-1</f>
         <v>71.799999279999938</v>
       </c>
-      <c r="K4" s="5">
+      <c r="Q4" s="10">
+        <f>ABS(((4*(ROUND(P4,0)+1)/(A4*10^6*8)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.25000090000007497</v>
+      </c>
+      <c r="R4" s="5">
         <f>A4*10^6*16*(1/100000 - 1/1111111)/4-1</f>
         <v>144.59999855999988</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S4" s="10">
+        <f>ABS(((4*(ROUND(R4,0)+1)/(A4*10^6*16)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.25000090000007497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>6</v>
       </c>
@@ -544,36 +634,68 @@
         <f t="shared" ref="C5:C14" si="0">A5*10^6/(9600*16*4)-1</f>
         <v>8.765625</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" ref="D5:D14" si="1">A5*10^6*4/(9600*16*4)-1</f>
+      <c r="D5" s="10">
+        <f t="shared" ref="D5:D14" si="1">ABS(A5*10^6/(16*4*(ROUND(C5,0)+1))-9600)*100/9600</f>
+        <v>2.34375</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" ref="E5:E14" si="2">A5*10^6*4/(9600*16*4)-1</f>
         <v>38.0625</v>
       </c>
-      <c r="E5" s="4">
-        <f t="shared" ref="E5:E14" si="2">A5*10^6*8/(9600*16*4)-1</f>
+      <c r="F5" s="10">
+        <f t="shared" ref="F5:F14" si="3">ABS(A5*10^6*4/(16*4*(ROUND(E5,0)+1))-9600)*100/9600</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G14" si="4">A5*10^6*8/(9600*16*4)-1</f>
         <v>77.125</v>
       </c>
-      <c r="F5" s="5">
-        <f t="shared" ref="F5:F14" si="3">A5*10^6*16/(9600*16*4)-1</f>
+      <c r="H5" s="10">
+        <f t="shared" ref="H5:H14" si="5">ABS(A5*10^6*8/(16*4*(ROUND(G5,0)+1))-9600)*100/9600</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ref="I5:I14" si="6">A5*10^6*16/(9600*16*4)-1</f>
         <v>155.25</v>
       </c>
-      <c r="H5" s="2">
-        <f t="shared" ref="H5:H14" si="4">A5*10^6*(1/100000 - 1/1111111)/4-1</f>
+      <c r="J5" s="10">
+        <f t="shared" ref="J5:J14" si="7">ABS(A5*10^6*16/(16*4*(ROUND(I5,0)+1))-9600)*100/9600</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" ref="L5:L14" si="8">A5*10^6*(1/100000 - 1/1111111)/4-1</f>
         <v>12.649999864999989</v>
       </c>
-      <c r="I5" s="3">
-        <f t="shared" ref="I5:I14" si="5">A5*10^6*4*(1/100000 - 1/1111111)/4-1</f>
+      <c r="M5" s="10">
+        <f t="shared" ref="M5:M14" si="9">ABS(((4*(ROUND(L5,0)+1)/(A5*10^6)))+1/1111111-1/100000)*100000*100</f>
+        <v>2.3333342333334022</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" ref="N5:N14" si="10">A5*10^6*4*(1/100000 - 1/1111111)/4-1</f>
         <v>53.599999459999957</v>
       </c>
-      <c r="J5" s="4">
-        <f t="shared" ref="J5:J14" si="6">A5*10^6*8*(1/100000 - 1/1111111)/4-1</f>
+      <c r="O5" s="10">
+        <f t="shared" ref="O5:O14" si="11">ABS(((4*(ROUND(N5,0)+1)/(A5*10^6*4)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.66666756666674043</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" ref="P5:P14" si="12">A5*10^6*8*(1/100000 - 1/1111111)/4-1</f>
         <v>108.19999891999991</v>
       </c>
-      <c r="K5" s="5">
-        <f t="shared" ref="K5:K14" si="7">A5*10^6*16*(1/100000 - 1/1111111)/4-1</f>
+      <c r="Q5" s="10">
+        <f t="shared" ref="Q5:S14" si="13">ABS(((4*(ROUND(P5,0)+1)/(A5*10^6*8)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.16666576666659053</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" ref="R5:R14" si="14">A5*10^6*16*(1/100000 - 1/1111111)/4-1</f>
         <v>217.39999783999983</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S5" s="10">
+        <f t="shared" ref="S5:S14" si="15">ABS(((4*(ROUND(R5,0)+1)/(A5*10^6*16)))+1/1111111-1/100000)*100000*100</f>
+        <v>0.16666576666659053</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>7.3727999999999998</v>
       </c>
@@ -581,36 +703,68 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="E6" s="4">
-        <f t="shared" si="2"/>
+      <c r="F6" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
-      <c r="F6" s="5">
-        <f t="shared" si="3"/>
+      <c r="H6" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="6"/>
         <v>191</v>
       </c>
-      <c r="H6" s="2">
-        <f t="shared" si="4"/>
+      <c r="J6" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="8"/>
         <v>15.773119834111984</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" si="5"/>
+      <c r="M6" s="10">
+        <f t="shared" si="9"/>
+        <v>1.2309036777778548</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="10"/>
         <v>66.092479336447937</v>
       </c>
-      <c r="J6" s="4">
-        <f t="shared" si="6"/>
+      <c r="O6" s="10">
+        <f t="shared" si="11"/>
+        <v>0.12543312777770932</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="12"/>
         <v>133.18495867289587</v>
       </c>
-      <c r="K6" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q6" s="10">
+        <f t="shared" si="13"/>
+        <v>0.12543312777770932</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="14"/>
         <v>267.36991734579175</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S6" s="10">
+        <f t="shared" si="15"/>
+        <v>0.12543312777770932</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>8</v>
       </c>
@@ -618,36 +772,68 @@
         <f t="shared" si="0"/>
         <v>12.020833333333334</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="10">
         <f t="shared" si="1"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
         <v>51.083333333333336</v>
       </c>
-      <c r="E7" s="4">
-        <f t="shared" si="2"/>
+      <c r="F7" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="4"/>
         <v>103.16666666666667</v>
       </c>
-      <c r="F7" s="5">
-        <f t="shared" si="3"/>
+      <c r="H7" s="10">
+        <f t="shared" si="5"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="6"/>
         <v>207.33333333333334</v>
       </c>
-      <c r="H7" s="2">
-        <f t="shared" si="4"/>
+      <c r="J7" s="10">
+        <f t="shared" si="7"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="8"/>
         <v>17.199999819999984</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" si="5"/>
+      <c r="M7" s="10">
+        <f t="shared" si="9"/>
+        <v>0.99999909999992154</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="10"/>
         <v>71.799999279999938</v>
       </c>
-      <c r="J7" s="4">
-        <f t="shared" si="6"/>
+      <c r="O7" s="10">
+        <f t="shared" si="11"/>
+        <v>0.25000090000007497</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="12"/>
         <v>144.59999855999988</v>
       </c>
-      <c r="K7" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q7" s="10">
+        <f t="shared" si="13"/>
+        <v>0.25000090000007497</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="14"/>
         <v>290.19999711999975</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S7" s="10">
+        <f t="shared" si="15"/>
+        <v>6.2499099999915667E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>11.059200000000001</v>
       </c>
@@ -655,36 +841,68 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="10">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="E8" s="4">
-        <f t="shared" si="2"/>
+      <c r="F8" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="4"/>
         <v>143</v>
       </c>
-      <c r="F8" s="5">
-        <f t="shared" si="3"/>
+      <c r="H8" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="6"/>
         <v>287</v>
       </c>
-      <c r="H8" s="2">
-        <f t="shared" si="4"/>
+      <c r="J8" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="8"/>
         <v>24.159679751167978</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="5"/>
+      <c r="M8" s="10">
+        <f t="shared" si="9"/>
+        <v>0.57754539629622514</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="10"/>
         <v>99.638719004671913</v>
       </c>
-      <c r="J8" s="4">
-        <f t="shared" si="6"/>
+      <c r="O8" s="10">
+        <f t="shared" si="11"/>
+        <v>0.32667914074082344</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="12"/>
         <v>200.27743800934383</v>
       </c>
-      <c r="K8" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q8" s="10">
+        <f t="shared" si="13"/>
+        <v>0.12543312777770932</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="14"/>
         <v>401.55487601868765</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S8" s="10">
+        <f t="shared" si="15"/>
+        <v>0.10062300648155703</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -692,36 +910,68 @@
         <f t="shared" si="0"/>
         <v>18.53125</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="10">
         <f t="shared" si="1"/>
+        <v>2.34375</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="2"/>
         <v>77.125</v>
       </c>
-      <c r="E9" s="4">
-        <f t="shared" si="2"/>
+      <c r="F9" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="4"/>
         <v>155.25</v>
       </c>
-      <c r="F9" s="5">
-        <f t="shared" si="3"/>
+      <c r="H9" s="10">
+        <f t="shared" si="5"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="6"/>
         <v>311.5</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" si="4"/>
+      <c r="J9" s="10">
+        <f t="shared" si="7"/>
+        <v>0.15974440894567957</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="8"/>
         <v>26.299999729999978</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="5"/>
+      <c r="M9" s="10">
+        <f t="shared" si="9"/>
+        <v>0.99999909999992154</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="10"/>
         <v>108.19999891999991</v>
       </c>
-      <c r="J9" s="4">
-        <f t="shared" si="6"/>
+      <c r="O9" s="10">
+        <f t="shared" si="11"/>
+        <v>0.16666576666659053</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="12"/>
         <v>217.39999783999983</v>
       </c>
-      <c r="K9" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q9" s="10">
+        <f t="shared" si="13"/>
+        <v>0.16666576666659053</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="14"/>
         <v>435.79999567999965</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S9" s="10">
+        <f t="shared" si="15"/>
+        <v>4.1667566666742234E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>20</v>
       </c>
@@ -729,36 +979,68 @@
         <f t="shared" si="0"/>
         <v>31.552083333333336</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <f t="shared" si="1"/>
+        <v>1.3573232323232294</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="2"/>
         <v>129.20833333333334</v>
       </c>
-      <c r="E10" s="4">
-        <f t="shared" si="2"/>
+      <c r="F10" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="4"/>
         <v>259.41666666666669</v>
       </c>
-      <c r="F10" s="5">
-        <f t="shared" si="3"/>
+      <c r="H10" s="10">
+        <f t="shared" si="5"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="6"/>
         <v>519.83333333333337</v>
       </c>
-      <c r="H10" s="2">
-        <f t="shared" si="4"/>
+      <c r="J10" s="10">
+        <f t="shared" si="7"/>
+        <v>3.1989763275760197E-2</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="8"/>
         <v>44.499999549999963</v>
       </c>
-      <c r="I10" s="3">
-        <f t="shared" si="5"/>
+      <c r="M10" s="10">
+        <f t="shared" si="9"/>
+        <v>0.99999909999992154</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="10"/>
         <v>180.99999819999985</v>
       </c>
-      <c r="J10" s="4">
-        <f t="shared" si="6"/>
+      <c r="O10" s="10">
+        <f t="shared" si="11"/>
+        <v>9.0000006890979777E-7</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="12"/>
         <v>362.9999963999997</v>
       </c>
-      <c r="K10" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q10" s="10">
+        <f t="shared" si="13"/>
+        <v>9.0000006890979777E-7</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="14"/>
         <v>726.9999927999994</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S10" s="10">
+        <f t="shared" si="15"/>
+        <v>9.0000006890979777E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>24</v>
       </c>
@@ -766,36 +1048,68 @@
         <f t="shared" si="0"/>
         <v>38.0625</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="10">
         <f t="shared" si="1"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
         <v>155.25</v>
       </c>
-      <c r="E11" s="4">
-        <f t="shared" si="2"/>
+      <c r="F11" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="4"/>
         <v>311.5</v>
       </c>
-      <c r="F11" s="5">
-        <f t="shared" si="3"/>
+      <c r="H11" s="10">
+        <f t="shared" si="5"/>
+        <v>0.15974440894567957</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="6"/>
         <v>624</v>
       </c>
-      <c r="H11" s="2">
-        <f t="shared" si="4"/>
+      <c r="J11" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="8"/>
         <v>53.599999459999957</v>
       </c>
-      <c r="I11" s="3">
-        <f t="shared" si="5"/>
+      <c r="M11" s="10">
+        <f t="shared" si="9"/>
+        <v>0.66666756666674043</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="10"/>
         <v>217.39999783999983</v>
       </c>
-      <c r="J11" s="4">
-        <f t="shared" si="6"/>
+      <c r="O11" s="10">
+        <f t="shared" si="11"/>
+        <v>0.16666576666659053</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="12"/>
         <v>435.79999567999965</v>
       </c>
-      <c r="K11" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q11" s="10">
+        <f t="shared" si="13"/>
+        <v>4.1667566666742234E-2</v>
+      </c>
+      <c r="R11" s="5">
+        <f t="shared" si="14"/>
         <v>872.59999135999931</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S11" s="10">
+        <f t="shared" si="15"/>
+        <v>4.1667566666742234E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>25</v>
       </c>
@@ -803,36 +1117,68 @@
         <f t="shared" si="0"/>
         <v>39.690104166666664</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="10">
         <f t="shared" si="1"/>
+        <v>0.75584349593496347</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="2"/>
         <v>161.76041666666666</v>
       </c>
-      <c r="E12" s="4">
-        <f t="shared" si="2"/>
+      <c r="F12" s="10">
+        <f t="shared" si="3"/>
+        <v>0.14698364008179018</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="4"/>
         <v>324.52083333333331</v>
       </c>
-      <c r="F12" s="5">
-        <f t="shared" si="3"/>
+      <c r="H12" s="10">
+        <f t="shared" si="5"/>
+        <v>0.14698364008179018</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="6"/>
         <v>650.04166666666663</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" si="4"/>
+      <c r="J12" s="10">
+        <f t="shared" si="7"/>
+        <v>6.4004096262237908E-3</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="8"/>
         <v>55.874999437499952</v>
       </c>
-      <c r="I12" s="3">
-        <f t="shared" si="5"/>
+      <c r="M12" s="10">
+        <f t="shared" si="9"/>
+        <v>0.20000090000008391</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="10"/>
         <v>226.49999774999981</v>
       </c>
-      <c r="J12" s="4">
-        <f t="shared" si="6"/>
+      <c r="O12" s="10">
+        <f t="shared" si="11"/>
+        <v>0.19999909999992918</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="12"/>
         <v>453.99999549999961</v>
       </c>
-      <c r="K12" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q12" s="10">
+        <f t="shared" si="13"/>
+        <v>9.0000006890979777E-7</v>
+      </c>
+      <c r="R12" s="5">
+        <f t="shared" si="14"/>
         <v>908.99999099999923</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S12" s="10">
+        <f t="shared" si="15"/>
+        <v>9.0000006890979777E-7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>32.768000000000001</v>
       </c>
@@ -840,36 +1186,68 @@
         <f t="shared" si="0"/>
         <v>52.333333333333336</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="10">
         <f t="shared" si="1"/>
+        <v>0.62893081761006897</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="2"/>
         <v>212.33333333333334</v>
       </c>
-      <c r="E13" s="4">
-        <f t="shared" si="2"/>
+      <c r="F13" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1564945226917113</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="4"/>
         <v>425.66666666666669</v>
       </c>
-      <c r="F13" s="5">
-        <f t="shared" si="3"/>
+      <c r="H13" s="10">
+        <f t="shared" si="5"/>
+        <v>7.806401249024475E-2</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="6"/>
         <v>852.33333333333337</v>
       </c>
-      <c r="H13" s="2">
-        <f t="shared" si="4"/>
+      <c r="J13" s="10">
+        <f t="shared" si="7"/>
+        <v>3.9077764751861345E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="8"/>
         <v>73.547199262719943</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="5"/>
+      <c r="M13" s="10">
+        <f t="shared" si="9"/>
+        <v>0.5527352750000728</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="10"/>
         <v>297.18879705087977</v>
       </c>
-      <c r="J13" s="4">
-        <f t="shared" si="6"/>
+      <c r="O13" s="10">
+        <f t="shared" si="11"/>
+        <v>5.7616287499927733E-2</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="12"/>
         <v>595.37759410175954</v>
       </c>
-      <c r="K13" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q13" s="10">
+        <f t="shared" si="13"/>
+        <v>5.7616287499927733E-2</v>
+      </c>
+      <c r="R13" s="5">
+        <f t="shared" si="14"/>
         <v>1191.7551882035191</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S13" s="10">
+        <f t="shared" si="15"/>
+        <v>1.8677657812580812E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>32</v>
       </c>
@@ -877,53 +1255,93 @@
         <f t="shared" si="0"/>
         <v>51.083333333333336</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="10">
         <f t="shared" si="1"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
         <v>207.33333333333334</v>
       </c>
-      <c r="E14" s="4">
-        <f t="shared" si="2"/>
+      <c r="F14" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="4"/>
         <v>415.66666666666669</v>
       </c>
-      <c r="F14" s="5">
-        <f t="shared" si="3"/>
+      <c r="H14" s="10">
+        <f t="shared" si="5"/>
+        <v>7.9936051159071056E-2</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="6"/>
         <v>832.33333333333337</v>
       </c>
-      <c r="H14" s="2">
-        <f t="shared" si="4"/>
+      <c r="J14" s="10">
+        <f t="shared" si="7"/>
+        <v>4.0016006402557501E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="8"/>
         <v>71.799999279999938</v>
       </c>
-      <c r="I14" s="3">
-        <f t="shared" si="5"/>
+      <c r="M14" s="10">
+        <f t="shared" si="9"/>
+        <v>0.25000090000007497</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="10"/>
         <v>290.19999711999975</v>
       </c>
-      <c r="J14" s="4">
-        <f t="shared" si="6"/>
+      <c r="O14" s="10">
+        <f t="shared" si="11"/>
+        <v>6.2499099999915667E-2</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="12"/>
         <v>581.3999942399995</v>
       </c>
-      <c r="K14" s="5">
-        <f t="shared" si="7"/>
+      <c r="Q14" s="10">
+        <f t="shared" si="13"/>
+        <v>6.2499099999915667E-2</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="14"/>
         <v>1163.799988479999</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="S14" s="10">
+        <f t="shared" si="15"/>
+        <v>1.5625900000077759E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -931,227 +1349,404 @@
         <f>A17*10^6/(38400*16*4)-1</f>
         <v>0.62760416666666674</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="10">
+        <f>ABS(A17*10^6/(16*4*(ROUND(C17,0)+1))-38400)*100/38400</f>
+        <v>18.619791666666668</v>
+      </c>
+      <c r="E17" s="3">
         <f>A17*10^6*4/(38400*16*4)-1</f>
         <v>5.510416666666667</v>
       </c>
-      <c r="E17" s="4">
+      <c r="F17" s="10">
+        <f>ABS(A17*10^6*4/(16*4*(ROUND(E17,0)+1))-38400)*100/38400</f>
+        <v>6.9940476190476115</v>
+      </c>
+      <c r="G17" s="4">
         <f>A17*10^6*8/(38400*16*4)-1</f>
         <v>12.020833333333334</v>
       </c>
-      <c r="F17" s="5">
+      <c r="H17" s="10">
+        <f>ABS(A17*10^6*8/(16*4*(ROUND(G17,0)+1))-38400)*100/38400</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I17" s="5">
         <f>A17*10^6*16/(38400*16*4)-1</f>
         <v>25.041666666666668</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J17" s="10">
+        <f>ABS(A17*10^6*16/(16*4*(ROUND(I17,0)+1))-38400)*100/38400</f>
+        <v>0.1602564102564088</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>6</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:C27" si="8">A18*10^6/(38400*16*4)-1</f>
+        <f t="shared" ref="C18:C27" si="16">A18*10^6/(38400*16*4)-1</f>
         <v>1.44140625</v>
       </c>
-      <c r="D18" s="3">
-        <f t="shared" ref="D18:D27" si="9">A18*10^6*4/(38400*16*4)-1</f>
+      <c r="D18" s="10">
+        <f t="shared" ref="D18:H27" si="17">ABS(A18*10^6/(16*4*(ROUND(C18,0)+1))-38400)*100/38400</f>
+        <v>22.0703125</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" ref="E18:E27" si="18">A18*10^6*4/(38400*16*4)-1</f>
         <v>8.765625</v>
       </c>
-      <c r="E18" s="4">
-        <f t="shared" ref="E18:E27" si="10">A18*10^6*8/(38400*16*4)-1</f>
+      <c r="F18" s="10">
+        <f t="shared" ref="F18:F27" si="19">ABS(A18*10^6*4/(16*4*(ROUND(E18,0)+1))-38400)*100/38400</f>
+        <v>2.34375</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" ref="G18:G27" si="20">A18*10^6*8/(38400*16*4)-1</f>
         <v>18.53125</v>
       </c>
-      <c r="F18" s="5">
-        <f t="shared" ref="F18:F27" si="11">A18*10^6*16/(38400*16*4)-1</f>
+      <c r="H18" s="10">
+        <f t="shared" ref="H18:J27" si="21">ABS(A18*10^6*8/(16*4*(ROUND(G18,0)+1))-38400)*100/38400</f>
+        <v>2.34375</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" ref="I18:I27" si="22">A18*10^6*16/(38400*16*4)-1</f>
         <v>38.0625</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J18" s="10">
+        <f t="shared" ref="J18:J27" si="23">ABS(A18*10^6*16/(16*4*(ROUND(I18,0)+1))-38400)*100/38400</f>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>7.3727999999999998</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
-      <c r="D19" s="3">
-        <f t="shared" si="9"/>
+      <c r="D19" s="10">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="E19" s="4">
-        <f t="shared" si="10"/>
+      <c r="F19" s="10">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="20"/>
         <v>23</v>
       </c>
-      <c r="F19" s="5">
-        <f t="shared" si="11"/>
+      <c r="H19" s="10">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J19" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>8</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>2.2552083333333335</v>
       </c>
-      <c r="D20" s="3">
-        <f t="shared" si="9"/>
+      <c r="D20" s="10">
+        <f t="shared" si="17"/>
+        <v>8.5069444444444375</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="18"/>
         <v>12.020833333333334</v>
       </c>
-      <c r="E20" s="4">
-        <f t="shared" si="10"/>
+      <c r="F20" s="10">
+        <f t="shared" si="19"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="20"/>
         <v>25.041666666666668</v>
       </c>
-      <c r="F20" s="5">
-        <f t="shared" si="11"/>
+      <c r="H20" s="10">
+        <f t="shared" si="21"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" si="22"/>
         <v>51.083333333333336</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J20" s="10">
+        <f t="shared" si="23"/>
+        <v>0.1602564102564088</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>11.059200000000001</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.5</v>
       </c>
-      <c r="D21" s="3">
-        <f t="shared" si="9"/>
+      <c r="D21" s="10">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
-      <c r="E21" s="4">
-        <f t="shared" si="10"/>
+      <c r="F21" s="10">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="20"/>
         <v>35</v>
       </c>
-      <c r="F21" s="5">
-        <f t="shared" si="11"/>
+      <c r="H21" s="10">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="22"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J21" s="10">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>12</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.8828125</v>
       </c>
-      <c r="D22" s="3">
-        <f t="shared" si="9"/>
+      <c r="D22" s="10">
+        <f t="shared" si="17"/>
+        <v>2.34375</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="18"/>
         <v>18.53125</v>
       </c>
-      <c r="E22" s="4">
-        <f t="shared" si="10"/>
+      <c r="F22" s="10">
+        <f t="shared" si="19"/>
+        <v>2.34375</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="20"/>
         <v>38.0625</v>
       </c>
-      <c r="F22" s="5">
-        <f t="shared" si="11"/>
+      <c r="H22" s="10">
+        <f t="shared" si="21"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="22"/>
         <v>77.125</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J22" s="10">
+        <f t="shared" si="23"/>
+        <v>0.1602564102564088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>7.1380208333333339</v>
       </c>
-      <c r="D23" s="3">
-        <f t="shared" si="9"/>
+      <c r="D23" s="10">
+        <f t="shared" si="17"/>
+        <v>1.7252604166666667</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="18"/>
         <v>31.552083333333336</v>
       </c>
-      <c r="E23" s="4">
-        <f t="shared" si="10"/>
+      <c r="F23" s="10">
+        <f t="shared" si="19"/>
+        <v>1.3573232323232294</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="20"/>
         <v>64.104166666666671</v>
       </c>
-      <c r="F23" s="5">
-        <f t="shared" si="11"/>
+      <c r="H23" s="10">
+        <f t="shared" si="21"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="22"/>
         <v>129.20833333333334</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J23" s="10">
+        <f t="shared" si="23"/>
+        <v>0.1602564102564088</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>24</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>8.765625</v>
       </c>
-      <c r="D24" s="3">
-        <f t="shared" si="9"/>
+      <c r="D24" s="10">
+        <f t="shared" si="17"/>
+        <v>2.34375</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="18"/>
         <v>38.0625</v>
       </c>
-      <c r="E24" s="4">
-        <f t="shared" si="10"/>
+      <c r="F24" s="10">
+        <f t="shared" si="19"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="20"/>
         <v>77.125</v>
       </c>
-      <c r="F24" s="5">
-        <f t="shared" si="11"/>
+      <c r="H24" s="10">
+        <f t="shared" si="21"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="22"/>
         <v>155.25</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J24" s="10">
+        <f t="shared" si="23"/>
+        <v>0.1602564102564088</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>25</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>9.1725260416666661</v>
       </c>
-      <c r="D25" s="3">
-        <f t="shared" si="9"/>
+      <c r="D25" s="10">
+        <f t="shared" si="17"/>
+        <v>1.7252604166666667</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="18"/>
         <v>39.690104166666664</v>
       </c>
-      <c r="E25" s="4">
-        <f t="shared" si="10"/>
+      <c r="F25" s="10">
+        <f t="shared" si="19"/>
+        <v>0.75584349593496347</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="20"/>
         <v>80.380208333333329</v>
       </c>
-      <c r="F25" s="5">
-        <f t="shared" si="11"/>
+      <c r="H25" s="10">
+        <f t="shared" si="21"/>
+        <v>0.46939300411522328</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="22"/>
         <v>161.76041666666666</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J25" s="10">
+        <f t="shared" si="23"/>
+        <v>0.14698364008179018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>32.768000000000001</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>12.333333333333334</v>
       </c>
-      <c r="D26" s="3">
-        <f t="shared" si="9"/>
+      <c r="D26" s="10">
+        <f t="shared" si="17"/>
+        <v>2.5641025641025599</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="18"/>
         <v>52.333333333333336</v>
       </c>
-      <c r="E26" s="4">
-        <f t="shared" si="10"/>
+      <c r="F26" s="10">
+        <f t="shared" si="19"/>
+        <v>0.62893081761006897</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="20"/>
         <v>105.66666666666667</v>
       </c>
-      <c r="F26" s="5">
-        <f t="shared" si="11"/>
+      <c r="H26" s="10">
+        <f t="shared" si="21"/>
+        <v>0.31152647975077724</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="22"/>
         <v>212.33333333333334</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J26" s="10">
+        <f t="shared" si="23"/>
+        <v>0.1564945226917113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>32</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>12.020833333333334</v>
       </c>
-      <c r="D27" s="3">
-        <f t="shared" si="9"/>
+      <c r="D27" s="10">
+        <f t="shared" si="17"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="18"/>
         <v>51.083333333333336</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" si="10"/>
+      <c r="F27" s="10">
+        <f t="shared" si="19"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="20"/>
         <v>103.16666666666667</v>
       </c>
-      <c r="F27" s="5">
-        <f t="shared" si="11"/>
+      <c r="H27" s="10">
+        <f t="shared" si="21"/>
+        <v>0.1602564102564088</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="22"/>
         <v>207.33333333333334</v>
+      </c>
+      <c r="J27" s="10">
+        <f t="shared" si="23"/>
+        <v>0.1602564102564088</v>
       </c>
     </row>
   </sheetData>
@@ -1159,8 +1754,8 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="L1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1171,7 +1766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>